<commit_message>
added day 14 and pushing day 11 and 12 changes
</commit_message>
<xml_diff>
--- a/day11/ProccedEmployeeData.xlsx
+++ b/day11/ProccedEmployeeData.xlsx
@@ -397,14 +397,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v xml:space="preserve">EmployeeID </v>
+        <v>EmployeeID</v>
       </c>
       <c r="B1" t="str">
         <v>AnnualSalary</v>
@@ -418,217 +418,287 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Worker 1</v>
+        <v>EMP001</v>
       </c>
       <c r="B2">
-        <v>42000</v>
+        <v>32500</v>
       </c>
       <c r="C2" t="str">
         <v>5%</v>
       </c>
       <c r="D2" t="str">
-        <v>2100.00</v>
+        <v>1625.00</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Worker 2</v>
+        <v>EMP002</v>
       </c>
       <c r="B3">
-        <v>48000</v>
+        <v>35000</v>
       </c>
       <c r="C3" t="str">
         <v>5%</v>
       </c>
       <c r="D3" t="str">
-        <v>2400.00</v>
+        <v>1750.00</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Worker 3</v>
+        <v>EMP003</v>
       </c>
       <c r="B4">
-        <v>54000</v>
+        <v>37500</v>
       </c>
       <c r="C4" t="str">
-        <v>7%</v>
+        <v>5%</v>
       </c>
       <c r="D4" t="str">
-        <v>3780.00</v>
+        <v>1875.00</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Worker 4</v>
+        <v>EMP004</v>
       </c>
       <c r="B5">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C5" t="str">
-        <v>7%</v>
+        <v>5%</v>
       </c>
       <c r="D5" t="str">
-        <v>4200.00</v>
+        <v>2000.00</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Worker 5</v>
+        <v>EMP005</v>
       </c>
       <c r="B6">
-        <v>66000</v>
+        <v>42500</v>
       </c>
       <c r="C6" t="str">
-        <v>7%</v>
+        <v>5%</v>
       </c>
       <c r="D6" t="str">
-        <v>4620.00</v>
+        <v>2125.00</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Worker 6</v>
+        <v>EMP006</v>
       </c>
       <c r="B7">
-        <v>72000</v>
+        <v>45000</v>
       </c>
       <c r="C7" t="str">
-        <v>7%</v>
+        <v>5%</v>
       </c>
       <c r="D7" t="str">
-        <v>5040.00</v>
+        <v>2250.00</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Worker 7</v>
+        <v>EMP007</v>
       </c>
       <c r="B8">
-        <v>78000</v>
+        <v>47500</v>
       </c>
       <c r="C8" t="str">
-        <v>7%</v>
+        <v>5%</v>
       </c>
       <c r="D8" t="str">
-        <v>5460.00</v>
+        <v>2375.00</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Worker 8</v>
+        <v>EMP008</v>
       </c>
       <c r="B9">
-        <v>84000</v>
+        <v>50000</v>
       </c>
       <c r="C9" t="str">
         <v>7%</v>
       </c>
       <c r="D9" t="str">
-        <v>5880.00</v>
+        <v>3500.00</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Worker 9</v>
+        <v>EMP009</v>
       </c>
       <c r="B10">
-        <v>90000</v>
+        <v>52500</v>
       </c>
       <c r="C10" t="str">
         <v>7%</v>
       </c>
       <c r="D10" t="str">
-        <v>6300.00</v>
+        <v>3675.00</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Worker 10</v>
+        <v>EMP010</v>
       </c>
       <c r="B11">
-        <v>96000</v>
+        <v>55000</v>
       </c>
       <c r="C11" t="str">
         <v>7%</v>
       </c>
       <c r="D11" t="str">
-        <v>6720.00</v>
+        <v>3850.00</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Worker 11</v>
+        <v>EMP011</v>
       </c>
       <c r="B12">
-        <v>102000</v>
+        <v>57500</v>
       </c>
       <c r="C12" t="str">
-        <v>10%</v>
+        <v>7%</v>
       </c>
       <c r="D12" t="str">
-        <v>10200.00</v>
+        <v>4025.00</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Worker 12</v>
+        <v>EMP012</v>
       </c>
       <c r="B13">
-        <v>108000</v>
+        <v>60000</v>
       </c>
       <c r="C13" t="str">
-        <v>10%</v>
+        <v>7%</v>
       </c>
       <c r="D13" t="str">
-        <v>10800.00</v>
+        <v>4200.00</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Worker 13</v>
+        <v>EMP013</v>
       </c>
       <c r="B14">
-        <v>124000</v>
+        <v>62500</v>
       </c>
       <c r="C14" t="str">
-        <v>10%</v>
+        <v>7%</v>
       </c>
       <c r="D14" t="str">
-        <v>12400.00</v>
+        <v>4375.00</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Worker 14</v>
+        <v>EMP014</v>
       </c>
       <c r="B15">
-        <v>130000</v>
+        <v>65000</v>
       </c>
       <c r="C15" t="str">
-        <v>10%</v>
+        <v>7%</v>
       </c>
       <c r="D15" t="str">
-        <v>13000.00</v>
+        <v>4550.00</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Worker 15</v>
+        <v>EMP015</v>
       </c>
       <c r="B16">
-        <v>136000</v>
+        <v>67500</v>
       </c>
       <c r="C16" t="str">
-        <v>10%</v>
+        <v>7%</v>
       </c>
       <c r="D16" t="str">
-        <v>13600.00</v>
+        <v>4725.00</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>EMP016</v>
+      </c>
+      <c r="B17">
+        <v>70000</v>
+      </c>
+      <c r="C17" t="str">
+        <v>7%</v>
+      </c>
+      <c r="D17" t="str">
+        <v>4900.00</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>EMP017</v>
+      </c>
+      <c r="B18">
+        <v>72500</v>
+      </c>
+      <c r="C18" t="str">
+        <v>7%</v>
+      </c>
+      <c r="D18" t="str">
+        <v>5075.00</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>EMP018</v>
+      </c>
+      <c r="B19">
+        <v>75000</v>
+      </c>
+      <c r="C19" t="str">
+        <v>7%</v>
+      </c>
+      <c r="D19" t="str">
+        <v>5250.00</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>EMP019</v>
+      </c>
+      <c r="B20">
+        <v>77500</v>
+      </c>
+      <c r="C20" t="str">
+        <v>7%</v>
+      </c>
+      <c r="D20" t="str">
+        <v>5425.00</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>EMP020</v>
+      </c>
+      <c r="B21">
+        <v>80000</v>
+      </c>
+      <c r="C21" t="str">
+        <v>7%</v>
+      </c>
+      <c r="D21" t="str">
+        <v>5600.00</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>